<commit_message>
tempadmindata template and file reading added.
</commit_message>
<xml_diff>
--- a/web/upload/Book1.xlsx
+++ b/web/upload/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HEP-KPU\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\poliodb\web\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,19 +24,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>nawid</t>
+    <t>par</t>
   </si>
   <si>
-    <t>nawid@gmail.com</t>
+    <t>two</t>
+  </si>
+  <si>
+    <t>gar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   two</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,24 +53,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -69,17 +82,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,29 +415,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>101</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G1" s="2">
+        <v>500</v>
+      </c>
+      <c r="H1" s="2">
+        <v>400</v>
+      </c>
+      <c r="I1" s="2">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2">
+        <v>60</v>
+      </c>
+      <c r="L1" s="2">
+        <v>50</v>
+      </c>
+      <c r="M1" s="2">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>50</v>
+      </c>
+      <c r="R1" s="2">
+        <v>3</v>
+      </c>
+      <c r="S1" s="3">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>102</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5">
+        <v>500</v>
+      </c>
+      <c r="G2" s="5">
+        <v>500</v>
+      </c>
+      <c r="H2" s="5">
+        <v>200</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>3</v>
+      </c>
+      <c r="K2" s="5">
+        <v>60</v>
+      </c>
+      <c r="L2" s="5">
+        <v>50</v>
+      </c>
+      <c r="M2" s="5">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5">
+        <v>30</v>
+      </c>
+      <c r="O2" s="5">
+        <v>20</v>
+      </c>
+      <c r="P2" s="5">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>50</v>
+      </c>
+      <c r="R2" s="5">
+        <v>3</v>
+      </c>
+      <c r="S2" s="6">
+        <v>2007</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>